<commit_message>
input time slots modified
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CSE\3-2\CSE-3203 (Algorithm 2)\Assignments\backtracking-class-routine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0326297-8659-4B7A-BAC3-0DE96B93F750}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E1179A-8D12-4456-A360-2EB5B89BFCD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="615" windowWidth="21600" windowHeight="12435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UndergradCurriculum" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="240">
   <si>
     <t>Semester</t>
   </si>
@@ -748,6 +748,9 @@
   </si>
   <si>
     <t>9:00am-1:00pm;2:00pm-5:00pm</t>
+  </si>
+  <si>
+    <t>10:00am-11:30pm</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1006"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -4401,7 +4404,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4485,17 +4488,15 @@
         <v>77</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="11" t="s">
         <v>35</v>
       </c>
+      <c r="C7" s="23" t="s">
+        <v>128</v>
+      </c>
       <c r="D7" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="23" t="s">
         <v>129</v>
       </c>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="10" t="s">
@@ -4665,6 +4666,9 @@
       </c>
       <c r="D20" s="13" t="s">
         <v>143</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4759,7 +4763,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5014,7 +5018,7 @@
         <v>156</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>156</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -5128,7 +5132,7 @@
         <v>110</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E22" s="24" t="s">
         <v>238</v>
@@ -5145,7 +5149,9 @@
         <v>144</v>
       </c>
       <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
+      <c r="D23" s="16" t="s">
+        <v>153</v>
+      </c>
       <c r="E23" s="24" t="s">
         <v>168</v>
       </c>

</xml_diff>

<commit_message>
Input file changed. Minor bug fix
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CSE\3-2\CSE-3203 (Algorithm 2)\Assignments\backtracking-class-routine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C13FC5-8E1E-4F5B-A7A5-FB5D03869AAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FC2DC9-B23D-4B92-9FC2-F93AA716C718}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UndergradCurriculum" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="232">
   <si>
     <t>Semester</t>
   </si>
@@ -507,15 +507,9 @@
     <t>2:00pm-3:30pm</t>
   </si>
   <si>
-    <t>8:30am-1:00am</t>
-  </si>
-  <si>
     <t>10:00am-11:30am</t>
   </si>
   <si>
-    <t>9:30am-1:00pm</t>
-  </si>
-  <si>
     <t>8:30am-1:00pm</t>
   </si>
   <si>
@@ -531,12 +525,6 @@
     <t>11:30am-1:00pm;2:00pm-5:00pm</t>
   </si>
   <si>
-    <t>9:00am-1:00pm</t>
-  </si>
-  <si>
-    <t>10:30am-1:00pm;2:00pm-5:00pm</t>
-  </si>
-  <si>
     <t>8:30am-1:00pm;2:00pm-5:00pm</t>
   </si>
   <si>
@@ -736,15 +724,6 @@
   </si>
   <si>
     <t>CHE 1114 Section 2</t>
-  </si>
-  <si>
-    <t>8:30am-12:00am;2:00pm-5:00pm</t>
-  </si>
-  <si>
-    <t>9:00am-1:00pm;2:00pm-5:00pm</t>
-  </si>
-  <si>
-    <t>10:00am-11:30pm</t>
   </si>
   <si>
     <t>8:30am-10:00am;2:00pm-5:00pm</t>
@@ -754,7 +733,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -812,11 +791,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -851,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -887,12 +861,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -902,8 +872,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4401,7 +4369,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4438,10 +4406,10 @@
       <c r="A2" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4449,10 +4417,10 @@
       <c r="A3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="21" t="s">
         <v>25</v>
       </c>
     </row>
@@ -4463,7 +4431,7 @@
       <c r="B4" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4487,13 +4455,13 @@
       <c r="B7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="10" t="s">
@@ -4510,7 +4478,7 @@
       <c r="B9" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="21" t="s">
         <v>131</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -4529,7 +4497,7 @@
       <c r="B11" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="21" t="s">
         <v>133</v>
       </c>
     </row>
@@ -4554,7 +4522,7 @@
       <c r="B13" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="21" t="s">
         <v>136</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -4587,7 +4555,7 @@
       <c r="B16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="21" t="s">
         <v>135</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -4622,7 +4590,7 @@
       <c r="B18" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="21" t="s">
         <v>139</v>
       </c>
       <c r="D18" s="11" t="s">
@@ -4636,7 +4604,7 @@
       <c r="A19" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -4733,11 +4701,11 @@
       <c r="B24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>234</v>
+      <c r="C24" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -4757,42 +4725,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA299A5-3E2F-4ACE-990F-4B04208826C9}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" customWidth="1"/>
     <col min="7" max="7" width="31.140625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>151</v>
       </c>
       <c r="H1" s="6" t="s">
@@ -4800,386 +4768,324 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="G7" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G21" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="G22" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="24" t="s">
+      <c r="F23" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>153</v>
+      <c r="F25" s="11" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -5191,8 +5097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="A1:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5242,7 +5148,7 @@
         <v>156</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1">
@@ -5264,7 +5170,7 @@
         <v>71</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>156</v>
@@ -5280,10 +5186,10 @@
         <v>75</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
@@ -5291,10 +5197,10 @@
         <v>77</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>153</v>
@@ -5316,16 +5222,16 @@
         <v>81</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>155</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1">
@@ -5338,7 +5244,7 @@
         <v>85</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.25" customHeight="1">
@@ -5363,10 +5269,10 @@
         <v>89</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>155</v>
@@ -5391,10 +5297,10 @@
         <v>94</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.25" customHeight="1">
@@ -5402,13 +5308,13 @@
         <v>96</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>155</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1">
@@ -5416,13 +5322,13 @@
         <v>99</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>155</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>157</v>
@@ -5442,7 +5348,7 @@
         <v>153</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1">
@@ -5450,13 +5356,13 @@
         <v>103</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>155</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
@@ -5473,37 +5379,37 @@
         <v>153</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G21" s="16" t="s">
-        <v>162</v>
+      <c r="G21" s="15" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1">
       <c r="A22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>162</v>
+      <c r="C22" s="16" t="s">
+        <v>160</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>153</v>
@@ -5524,10 +5430,10 @@
         <v>155</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1">
@@ -5535,13 +5441,13 @@
         <v>114</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>154</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1">
@@ -5549,10 +5455,10 @@
         <v>116</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.25" customHeight="1"/>
@@ -7284,7 +7190,7 @@
     <row r="67" spans="1:3" ht="13.5" customHeight="1">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C67" s="4">
         <v>3</v>
@@ -7293,7 +7199,7 @@
     <row r="68" spans="1:3" ht="13.5" customHeight="1">
       <c r="A68" s="3"/>
       <c r="B68" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C68" s="4">
         <v>3</v>
@@ -7302,7 +7208,7 @@
     <row r="69" spans="1:3" ht="13.5" customHeight="1">
       <c r="A69" s="4"/>
       <c r="B69" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C69" s="4">
         <v>3</v>
@@ -7311,7 +7217,7 @@
     <row r="70" spans="1:3" ht="13.5" customHeight="1">
       <c r="A70" s="4"/>
       <c r="B70" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C70" s="4">
         <v>3</v>
@@ -7320,7 +7226,7 @@
     <row r="71" spans="1:3" ht="13.5" customHeight="1">
       <c r="A71" s="4"/>
       <c r="B71" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C71" s="4">
         <v>3</v>
@@ -7329,7 +7235,7 @@
     <row r="72" spans="1:3" ht="13.5" customHeight="1">
       <c r="A72" s="4"/>
       <c r="B72" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C72" s="4">
         <v>3</v>
@@ -7338,7 +7244,7 @@
     <row r="73" spans="1:3" ht="13.5" customHeight="1">
       <c r="A73" s="4"/>
       <c r="B73" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C73" s="4">
         <v>3</v>
@@ -7347,7 +7253,7 @@
     <row r="74" spans="1:3" ht="13.5" customHeight="1">
       <c r="A74" s="4"/>
       <c r="B74" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C74" s="4">
         <v>3</v>
@@ -7374,7 +7280,7 @@
     <row r="77" spans="1:3" ht="13.5" customHeight="1">
       <c r="A77" s="4"/>
       <c r="B77" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C77" s="4">
         <v>1.5</v>
@@ -7383,7 +7289,7 @@
     <row r="78" spans="1:3" ht="13.5" customHeight="1">
       <c r="A78" s="4"/>
       <c r="B78" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C78" s="4">
         <v>1.5</v>
@@ -7392,7 +7298,7 @@
     <row r="79" spans="1:3" ht="13.5" customHeight="1">
       <c r="A79" s="4"/>
       <c r="B79" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C79" s="4">
         <v>1.5</v>
@@ -7401,7 +7307,7 @@
     <row r="80" spans="1:3" ht="13.5" customHeight="1">
       <c r="A80" s="4"/>
       <c r="B80" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C80" s="4">
         <v>1.5</v>
@@ -7410,7 +7316,7 @@
     <row r="81" spans="1:3" ht="13.5" customHeight="1">
       <c r="A81" s="4"/>
       <c r="B81" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C81" s="4">
         <v>1.5</v>
@@ -7419,7 +7325,7 @@
     <row r="82" spans="1:3" ht="13.5" customHeight="1">
       <c r="A82" s="4"/>
       <c r="B82" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C82" s="4">
         <v>1.5</v>
@@ -7428,7 +7334,7 @@
     <row r="83" spans="1:3" ht="13.5" customHeight="1">
       <c r="A83" s="4"/>
       <c r="B83" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C83" s="4">
         <v>1.5</v>
@@ -7437,7 +7343,7 @@
     <row r="84" spans="1:3" ht="13.5" customHeight="1">
       <c r="A84" s="4"/>
       <c r="B84" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C84" s="4">
         <v>1.5</v>
@@ -7464,7 +7370,7 @@
     <row r="87" spans="1:3" ht="13.5" customHeight="1">
       <c r="A87" s="4"/>
       <c r="B87" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C87" s="4">
         <v>3</v>
@@ -7473,7 +7379,7 @@
     <row r="88" spans="1:3" ht="13.5" customHeight="1">
       <c r="A88" s="4"/>
       <c r="B88" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C88" s="4">
         <v>3</v>
@@ -7491,7 +7397,7 @@
     <row r="90" spans="1:3" ht="13.5" customHeight="1">
       <c r="A90" s="4"/>
       <c r="B90" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C90" s="4">
         <v>3</v>
@@ -7500,7 +7406,7 @@
     <row r="91" spans="1:3" ht="13.5" customHeight="1">
       <c r="A91" s="4"/>
       <c r="B91" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C91" s="4">
         <v>3</v>
@@ -7509,7 +7415,7 @@
     <row r="92" spans="1:3" ht="13.5" customHeight="1">
       <c r="A92" s="4"/>
       <c r="B92" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C92" s="4">
         <v>3</v>
@@ -7527,7 +7433,7 @@
     <row r="94" spans="1:3" ht="13.5" customHeight="1">
       <c r="A94" s="4"/>
       <c r="B94" s="4" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C94" s="4">
         <v>3</v>
@@ -7536,7 +7442,7 @@
     <row r="95" spans="1:3" ht="13.5" customHeight="1">
       <c r="A95" s="4"/>
       <c r="B95" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C95" s="4">
         <v>3</v>
@@ -7545,7 +7451,7 @@
     <row r="96" spans="1:3" ht="13.5" customHeight="1">
       <c r="A96" s="4"/>
       <c r="B96" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C96" s="7">
         <v>3</v>
@@ -7554,7 +7460,7 @@
     <row r="97" spans="1:3" ht="13.5" customHeight="1">
       <c r="A97" s="4"/>
       <c r="B97" s="4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C97" s="8">
         <v>3</v>
@@ -7563,7 +7469,7 @@
     <row r="98" spans="1:3" ht="13.5" customHeight="1">
       <c r="A98" s="4"/>
       <c r="B98" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C98" s="7">
         <v>3</v>
@@ -7572,7 +7478,7 @@
     <row r="99" spans="1:3" ht="13.5" customHeight="1">
       <c r="A99" s="4"/>
       <c r="B99" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C99" s="7">
         <v>3</v>
@@ -7581,7 +7487,7 @@
     <row r="100" spans="1:3" ht="13.5" customHeight="1">
       <c r="A100" s="4"/>
       <c r="B100" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C100" s="7">
         <v>3</v>
@@ -7590,7 +7496,7 @@
     <row r="101" spans="1:3" ht="13.5" customHeight="1">
       <c r="A101" s="4"/>
       <c r="B101" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C101" s="7">
         <v>3</v>
@@ -7599,7 +7505,7 @@
     <row r="102" spans="1:3" ht="13.5" customHeight="1">
       <c r="A102" s="4"/>
       <c r="B102" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C102" s="7">
         <v>3</v>
@@ -7608,7 +7514,7 @@
     <row r="103" spans="1:3" ht="13.5" customHeight="1">
       <c r="A103" s="4"/>
       <c r="B103" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C103" s="7">
         <v>3</v>
@@ -7617,7 +7523,7 @@
     <row r="104" spans="1:3" ht="13.5" customHeight="1">
       <c r="A104" s="4"/>
       <c r="B104" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C104" s="7">
         <v>3</v>
@@ -7626,7 +7532,7 @@
     <row r="105" spans="1:3" ht="13.5" customHeight="1">
       <c r="A105" s="4"/>
       <c r="B105" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C105" s="7">
         <v>3</v>
@@ -7635,7 +7541,7 @@
     <row r="106" spans="1:3" ht="13.5" customHeight="1">
       <c r="A106" s="4"/>
       <c r="B106" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C106" s="7">
         <v>1.5</v>
@@ -7644,7 +7550,7 @@
     <row r="107" spans="1:3" ht="13.5" customHeight="1">
       <c r="A107" s="4"/>
       <c r="B107" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C107" s="7">
         <v>1.5</v>
@@ -7653,7 +7559,7 @@
     <row r="108" spans="1:3" ht="13.5" customHeight="1">
       <c r="A108" s="4"/>
       <c r="B108" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C108" s="7">
         <v>1.5</v>
@@ -7662,7 +7568,7 @@
     <row r="109" spans="1:3" ht="13.5" customHeight="1">
       <c r="A109" s="4"/>
       <c r="B109" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C109" s="7">
         <v>1.5</v>
@@ -7671,7 +7577,7 @@
     <row r="110" spans="1:3" ht="13.5" customHeight="1">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C110" s="7">
         <v>1.5</v>
@@ -7680,7 +7586,7 @@
     <row r="111" spans="1:3" ht="13.5" customHeight="1">
       <c r="A111" s="4"/>
       <c r="B111" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C111" s="7">
         <v>1.5</v>
@@ -7689,7 +7595,7 @@
     <row r="112" spans="1:3" ht="13.5" customHeight="1">
       <c r="A112" s="4"/>
       <c r="B112" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C112" s="7">
         <v>1.5</v>
@@ -7698,7 +7604,7 @@
     <row r="113" spans="1:3" ht="13.5" customHeight="1">
       <c r="A113" s="4"/>
       <c r="B113" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C113" s="7">
         <v>1.5</v>
@@ -7707,7 +7613,7 @@
     <row r="114" spans="1:3" ht="13.5" customHeight="1">
       <c r="A114" s="4"/>
       <c r="B114" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C114" s="7">
         <v>1.5</v>
@@ -7716,7 +7622,7 @@
     <row r="115" spans="1:3" ht="13.5" customHeight="1">
       <c r="A115" s="4"/>
       <c r="B115" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C115" s="7">
         <v>1.5</v>
@@ -7725,7 +7631,7 @@
     <row r="116" spans="1:3" ht="13.5" customHeight="1">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C116" s="7">
         <v>3</v>
@@ -7734,7 +7640,7 @@
     <row r="117" spans="1:3" ht="13.5" customHeight="1">
       <c r="A117" s="4"/>
       <c r="B117" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C117" s="7">
         <v>3</v>
@@ -7743,7 +7649,7 @@
     <row r="118" spans="1:3" ht="13.5" customHeight="1">
       <c r="A118" s="4"/>
       <c r="B118" s="4" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C118" s="7">
         <v>3</v>
@@ -7752,7 +7658,7 @@
     <row r="119" spans="1:3" ht="13.5" customHeight="1">
       <c r="A119" s="4"/>
       <c r="B119" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C119" s="7">
         <v>3</v>
@@ -7761,7 +7667,7 @@
     <row r="120" spans="1:3" ht="13.5" customHeight="1">
       <c r="A120" s="4"/>
       <c r="B120" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C120" s="7">
         <v>3</v>
@@ -7770,7 +7676,7 @@
     <row r="121" spans="1:3" ht="13.5" customHeight="1">
       <c r="A121" s="4"/>
       <c r="B121" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C121" s="7">
         <v>3</v>
@@ -7779,7 +7685,7 @@
     <row r="122" spans="1:3" ht="13.5" customHeight="1">
       <c r="A122" s="4"/>
       <c r="B122" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C122" s="7">
         <v>3</v>
@@ -7788,7 +7694,7 @@
     <row r="123" spans="1:3" ht="13.5" customHeight="1">
       <c r="A123" s="4"/>
       <c r="B123" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C123" s="7">
         <v>3</v>
@@ -7797,7 +7703,7 @@
     <row r="124" spans="1:3" ht="13.5" customHeight="1">
       <c r="A124" s="4"/>
       <c r="B124" s="4" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C124" s="7">
         <v>3</v>
@@ -7806,7 +7712,7 @@
     <row r="125" spans="1:3" ht="13.5" customHeight="1">
       <c r="A125" s="4"/>
       <c r="B125" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C125" s="7">
         <v>3</v>
@@ -7815,7 +7721,7 @@
     <row r="126" spans="1:3" ht="13.5" customHeight="1">
       <c r="A126" s="4"/>
       <c r="B126" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C126" s="7">
         <v>3</v>
@@ -7824,7 +7730,7 @@
     <row r="127" spans="1:3" ht="13.5" customHeight="1">
       <c r="A127" s="4"/>
       <c r="B127" s="4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C127" s="7">
         <v>3</v>
@@ -7833,7 +7739,7 @@
     <row r="128" spans="1:3" ht="13.5" customHeight="1">
       <c r="A128" s="4"/>
       <c r="B128" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C128" s="7">
         <v>3</v>
@@ -8786,7 +8692,7 @@
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1">
@@ -8811,7 +8717,7 @@
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1">
@@ -8836,7 +8742,7 @@
     </row>
     <row r="14" spans="1:8" ht="14.25" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.25" customHeight="1">
@@ -8861,7 +8767,7 @@
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
@@ -8873,25 +8779,25 @@
       <c r="A21" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="20" t="s">
-        <v>230</v>
+      <c r="C21" s="18" t="s">
+        <v>226</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C22" s="20"/>
+        <v>228</v>
+      </c>
+      <c r="C22" s="18"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -8902,16 +8808,16 @@
         <v>112</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>155</v>

</xml_diff>

<commit_message>
made sunday the first day and created routine list
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CSE\3-2\CSE-3203 (Algorithm 2)\Assignments\backtracking-class-routine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FC2DC9-B23D-4B92-9FC2-F93AA716C718}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A41FEFC-8FB9-4C74-B1B1-D807CE3E91AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UndergradCurriculum" sheetId="1" r:id="rId1"/>
@@ -4725,8 +4725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA299A5-3E2F-4ACE-990F-4B04208826C9}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4746,35 +4746,35 @@
         <v>118</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>163</v>
       </c>
     </row>
@@ -4782,13 +4782,13 @@
       <c r="A3" s="10" t="s">
         <v>69</v>
       </c>
+      <c r="B3" s="11" t="s">
+        <v>155</v>
+      </c>
       <c r="C3" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="11" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4796,10 +4796,10 @@
       <c r="A4" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4812,10 +4812,10 @@
       <c r="A6" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4823,16 +4823,16 @@
       <c r="A7" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>158</v>
       </c>
+      <c r="D7" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="E7" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G7" s="11" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4840,7 +4840,7 @@
       <c r="A8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="11" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4848,16 +4848,16 @@
       <c r="A9" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="13" t="s">
         <v>165</v>
       </c>
+      <c r="D9" s="11" t="s">
+        <v>160</v>
+      </c>
       <c r="E9" s="11" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G9" s="11" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4870,7 +4870,7 @@
       <c r="A11" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>161</v>
       </c>
     </row>
@@ -4878,16 +4878,16 @@
       <c r="A12" s="10" t="s">
         <v>87</v>
       </c>
+      <c r="B12" s="11" t="s">
+        <v>153</v>
+      </c>
       <c r="C12" s="11" t="s">
         <v>153</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="F12" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4895,16 +4895,16 @@
       <c r="A13" s="10" t="s">
         <v>89</v>
       </c>
+      <c r="C13" s="11" t="s">
+        <v>165</v>
+      </c>
       <c r="D13" s="11" t="s">
         <v>165</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G13" s="11" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4912,10 +4912,10 @@
       <c r="A14" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4923,10 +4923,10 @@
       <c r="A15" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4934,157 +4934,157 @@
       <c r="A16" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="11" t="s">
         <v>163</v>
       </c>
+      <c r="E16" s="11" t="s">
+        <v>155</v>
+      </c>
       <c r="F16" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G16" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:6">
       <c r="A17" s="10" t="s">
         <v>99</v>
       </c>
+      <c r="C17" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="D17" s="11" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G17" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:6">
       <c r="A18" s="10" t="s">
         <v>101</v>
       </c>
+      <c r="B18" s="11" t="s">
+        <v>153</v>
+      </c>
       <c r="C18" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>156</v>
-      </c>
       <c r="F18" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G18" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:6">
       <c r="A19" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:6">
       <c r="A20" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="D20" s="11" t="s">
+        <v>157</v>
+      </c>
       <c r="E20" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G20" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:6">
       <c r="A21" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="D21" s="11" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F21" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="F21" s="15" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:6">
       <c r="A22" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="B22" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="D22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="E22" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G22" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:6">
       <c r="A23" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13" t="s">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="F23" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:6">
       <c r="A24" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="F24" s="13" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:6">
       <c r="A25" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>158</v>
       </c>
     </row>
@@ -5098,7 +5098,7 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="A1:G25"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5119,35 +5119,35 @@
         <v>118</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5155,13 +5155,13 @@
       <c r="A3" s="9" t="s">
         <v>69</v>
       </c>
+      <c r="B3" s="11" t="s">
+        <v>155</v>
+      </c>
       <c r="C3" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" s="11" t="s">
         <v>157</v>
       </c>
     </row>
@@ -5169,10 +5169,10 @@
       <c r="A4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5185,10 +5185,10 @@
       <c r="A6" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>158</v>
       </c>
     </row>
@@ -5196,16 +5196,16 @@
       <c r="A7" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>158</v>
       </c>
+      <c r="D7" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="E7" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G7" s="11" t="s">
         <v>153</v>
       </c>
     </row>
@@ -5213,7 +5213,7 @@
       <c r="A8" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="11" t="s">
         <v>153</v>
       </c>
     </row>
@@ -5221,16 +5221,16 @@
       <c r="A9" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="12" t="s">
         <v>165</v>
       </c>
+      <c r="D9" s="11" t="s">
+        <v>160</v>
+      </c>
       <c r="E9" s="11" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G9" s="11" t="s">
         <v>158</v>
       </c>
     </row>
@@ -5243,7 +5243,7 @@
       <c r="A11" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>161</v>
       </c>
     </row>
@@ -5251,16 +5251,16 @@
       <c r="A12" s="9" t="s">
         <v>87</v>
       </c>
+      <c r="B12" s="11" t="s">
+        <v>153</v>
+      </c>
       <c r="C12" s="11" t="s">
         <v>153</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="F12" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5268,16 +5268,16 @@
       <c r="A13" s="9" t="s">
         <v>89</v>
       </c>
+      <c r="C13" s="11" t="s">
+        <v>165</v>
+      </c>
       <c r="D13" s="11" t="s">
         <v>165</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G13" s="11" t="s">
         <v>155</v>
       </c>
     </row>
@@ -5285,10 +5285,10 @@
       <c r="A14" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>156</v>
       </c>
     </row>
@@ -5296,10 +5296,10 @@
       <c r="A15" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="F15" s="11" t="s">
         <v>158</v>
       </c>
     </row>
@@ -5307,169 +5307,169 @@
       <c r="A16" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="11" t="s">
         <v>163</v>
       </c>
+      <c r="E16" s="11" t="s">
+        <v>155</v>
+      </c>
       <c r="F16" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G16" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="14.25" customHeight="1">
+    <row r="17" spans="1:6" ht="14.25" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>99</v>
       </c>
+      <c r="C17" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="D17" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G17" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="14.25" customHeight="1">
+    <row r="18" spans="1:6" ht="14.25" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>101</v>
       </c>
+      <c r="B18" s="11" t="s">
+        <v>153</v>
+      </c>
       <c r="C18" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>156</v>
-      </c>
       <c r="F18" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G18" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14.25" customHeight="1">
+    <row r="19" spans="1:6" ht="14.25" customHeight="1">
       <c r="A19" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="14.25" customHeight="1">
+    <row r="20" spans="1:6" ht="14.25" customHeight="1">
       <c r="A20" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="11" t="s">
         <v>153</v>
       </c>
+      <c r="D20" s="11" t="s">
+        <v>157</v>
+      </c>
       <c r="E20" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G20" s="11" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.25" customHeight="1">
+    <row r="21" spans="1:6" ht="14.25" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="D21" s="11" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F21" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="F21" s="15" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="14.25" customHeight="1">
+    <row r="22" spans="1:6" ht="14.25" customHeight="1">
       <c r="A22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="B22" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="D22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="11" t="s">
+        <v>158</v>
+      </c>
       <c r="E22" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G22" s="11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="14.25" customHeight="1">
+    <row r="23" spans="1:6" ht="14.25" customHeight="1">
       <c r="A23" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="E23" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="F23" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="14.25" customHeight="1">
+    <row r="24" spans="1:6" ht="14.25" customHeight="1">
       <c r="A24" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="B24" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="F24" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="14.25" customHeight="1">
+    <row r="25" spans="1:6" ht="14.25" customHeight="1">
       <c r="A25" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:7" ht="14.25" customHeight="1">
+    <row r="26" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:6" ht="14.25" customHeight="1">
       <c r="B28" s="12"/>
     </row>
-    <row r="29" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:7" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:7" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -6448,7 +6448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>